<commit_message>
amodified printscreen and checkboxes code
</commit_message>
<xml_diff>
--- a/TestData/RegistrationTest.xlsx
+++ b/TestData/RegistrationTest.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="28">
   <si>
     <t>Username</t>
   </si>
@@ -97,6 +97,9 @@
   </si>
   <si>
     <t>AgreeTerms</t>
+  </si>
+  <si>
+    <t>agreeTerms</t>
   </si>
 </sst>
 </file>
@@ -172,11 +175,14 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -475,7 +481,7 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -488,6 +494,7 @@
     <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -544,8 +551,8 @@
       <c r="H2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="1" t="b">
-        <v>1</v>
+      <c r="I2" s="4" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -573,8 +580,8 @@
       <c r="H3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I3" s="1" t="b">
-        <v>1</v>
+      <c r="I3" s="4" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -602,8 +609,8 @@
       <c r="H4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I4" s="1" t="b">
-        <v>0</v>
+      <c r="I4" s="4" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -631,8 +638,8 @@
       <c r="H5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I5" s="1" t="b">
-        <v>0</v>
+      <c r="I5" s="4" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -660,8 +667,8 @@
       <c r="H6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I6" s="1" t="b">
-        <v>1</v>
+      <c r="I6" s="4" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added new data driven excel code
</commit_message>
<xml_diff>
--- a/TestData/RegistrationTest.xlsx
+++ b/TestData/RegistrationTest.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2475" windowWidth="16020" windowHeight="6480"/>
+    <workbookView xWindow="0" yWindow="330" windowWidth="14550" windowHeight="3060"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,6 +12,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
+  <oleSize ref="A1:I8"/>
 </workbook>
 </file>
 
@@ -702,7 +703,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>

</xml_diff>